<commit_message>
Envisioning , I'm a data scientist :)
</commit_message>
<xml_diff>
--- a/Microsoft Excel/Tanvir/Day 02.xlsx
+++ b/Microsoft Excel/Tanvir/Day 02.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taroto/Documents/GitHub/Spreadsheet/Microsoft Excel/Tanvir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EB9A02-3A9B-834F-B6AB-06E8CE991DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CDBC09-5F80-014F-A3C1-1B4413FDFBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{9F8291B1-12C9-6E43-84E1-4C74E854AA37}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="18 Jan 2025" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088B1D09-73C6-BA48-A00A-52E28C9AF56E}">
   <dimension ref="B6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>